<commit_message>
subindo restante dos testes
</commit_message>
<xml_diff>
--- a/Feature02_criar_tarefa/CriarTarefa.xlsx
+++ b/Feature02_criar_tarefa/CriarTarefa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\Aulas Faculdade\ProjetoUC\Feature02_criar_tarefa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FC25F5-42AF-4699-B6C7-99D4C523BF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826A46AD-DAAA-43A1-8985-D93CA1C76723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>senha</t>
   </si>
   <si>
-    <t>Fernanda</t>
-  </si>
-  <si>
     <t>descrição</t>
   </si>
   <si>
@@ -94,7 +91,10 @@
     <t>teste_excedido.csv</t>
   </si>
   <si>
-    <t>81721367</t>
+    <t>Lorenzo Juliati</t>
+  </si>
+  <si>
+    <t>819221773</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>21</v>
@@ -508,54 +508,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -575,18 +575,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -606,24 +606,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -643,24 +643,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>